<commit_message>
Added more to the file return folder
</commit_message>
<xml_diff>
--- a/File Return Folder/DeformationMapsChallDataRemoved.xlsx
+++ b/File Return Folder/DeformationMapsChallDataRemoved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DROP\Dropbox (ORNL)\MBAAM_APS_SRP_Sim\SRPDrafts\SRP\SRPCALLPackage\Deformation\ChallTask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aahenri\Sandia_Project_Work\SRP_AM_Prediction_Challenge\File Return Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A77370D-28AB-41B4-A77E-4D7ADC78F447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B68C165-9416-4DAE-B252-A639A5945731}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1070" yWindow="-110" windowWidth="24640" windowHeight="14620" xr2:uid="{9EF05EA4-8B0F-466D-B13D-AFEA84469850}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9EF05EA4-8B0F-466D-B13D-AFEA84469850}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAL 4" sheetId="8" r:id="rId1"/>
@@ -1431,16 +1431,16 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1451,127 +1451,127 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-300</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-275</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-250</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-225</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-200</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-175</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-150</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-125</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-75</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>275</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>300</v>
       </c>

</xml_diff>